<commit_message>
Adding Los Angeles County data.
</commit_message>
<xml_diff>
--- a/Salt_Lake_Data.xlsx
+++ b/Salt_Lake_Data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="126">
   <si>
     <t>Unnamed: 0</t>
   </si>
@@ -97,6 +97,12 @@
     <t>Unnamed: 0.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1</t>
   </si>
   <si>
+    <t>Unnamed: 0.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1</t>
+  </si>
+  <si>
+    <t>Unnamed: 0.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1</t>
+  </si>
+  <si>
     <t>Date</t>
   </si>
   <si>
@@ -374,6 +380,18 @@
   </si>
   <si>
     <t>06-17-2020</t>
+  </si>
+  <si>
+    <t>06-18-2020</t>
+  </si>
+  <si>
+    <t>06-19-2020</t>
+  </si>
+  <si>
+    <t>06-20-2020</t>
+  </si>
+  <si>
+    <t>06-21-2020</t>
   </si>
 </sst>
 </file>
@@ -731,13 +749,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AG89"/>
+  <dimension ref="A1:AI93"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:33">
+    <row r="1" spans="1:35">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -834,8 +852,14 @@
       <c r="AG1" s="1" t="s">
         <v>31</v>
       </c>
+      <c r="AH1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>33</v>
+      </c>
     </row>
-    <row r="2" spans="1:33">
+    <row r="2" spans="1:35">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -920,23 +944,29 @@
       <c r="AB2">
         <v>0</v>
       </c>
-      <c r="AC2" t="s">
-        <v>32</v>
+      <c r="AC2">
+        <v>0</v>
       </c>
       <c r="AD2">
+        <v>0</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>34</v>
+      </c>
+      <c r="AF2">
         <v>80</v>
       </c>
-      <c r="AE2">
-        <v>0</v>
-      </c>
-      <c r="AF2">
-        <v>0</v>
-      </c>
       <c r="AG2">
         <v>0</v>
       </c>
+      <c r="AH2">
+        <v>0</v>
+      </c>
+      <c r="AI2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" spans="1:33">
+    <row r="3" spans="1:35">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1021,23 +1051,29 @@
       <c r="AB3">
         <v>1</v>
       </c>
-      <c r="AC3" t="s">
-        <v>33</v>
+      <c r="AC3">
+        <v>1</v>
       </c>
       <c r="AD3">
+        <v>1</v>
+      </c>
+      <c r="AE3" t="s">
+        <v>35</v>
+      </c>
+      <c r="AF3">
         <v>109</v>
       </c>
-      <c r="AE3">
-        <v>0</v>
-      </c>
-      <c r="AF3">
-        <v>0</v>
-      </c>
       <c r="AG3">
         <v>0</v>
       </c>
+      <c r="AH3">
+        <v>0</v>
+      </c>
+      <c r="AI3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="4" spans="1:33">
+    <row r="4" spans="1:35">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1122,23 +1158,29 @@
       <c r="AB4">
         <v>2</v>
       </c>
-      <c r="AC4" t="s">
-        <v>34</v>
+      <c r="AC4">
+        <v>2</v>
       </c>
       <c r="AD4">
+        <v>2</v>
+      </c>
+      <c r="AE4" t="s">
+        <v>36</v>
+      </c>
+      <c r="AF4">
         <v>124</v>
       </c>
-      <c r="AE4">
-        <v>0</v>
-      </c>
-      <c r="AF4">
-        <v>0</v>
-      </c>
       <c r="AG4">
         <v>0</v>
       </c>
+      <c r="AH4">
+        <v>0</v>
+      </c>
+      <c r="AI4">
+        <v>0</v>
+      </c>
     </row>
-    <row r="5" spans="1:33">
+    <row r="5" spans="1:35">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -1223,23 +1265,29 @@
       <c r="AB5">
         <v>3</v>
       </c>
-      <c r="AC5" t="s">
-        <v>35</v>
+      <c r="AC5">
+        <v>3</v>
       </c>
       <c r="AD5">
+        <v>3</v>
+      </c>
+      <c r="AE5" t="s">
+        <v>37</v>
+      </c>
+      <c r="AF5">
         <v>151</v>
       </c>
-      <c r="AE5">
-        <v>0</v>
-      </c>
-      <c r="AF5">
-        <v>0</v>
-      </c>
       <c r="AG5">
         <v>0</v>
       </c>
+      <c r="AH5">
+        <v>0</v>
+      </c>
+      <c r="AI5">
+        <v>0</v>
+      </c>
     </row>
-    <row r="6" spans="1:33">
+    <row r="6" spans="1:35">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -1324,23 +1372,29 @@
       <c r="AB6">
         <v>4</v>
       </c>
-      <c r="AC6" t="s">
-        <v>36</v>
+      <c r="AC6">
+        <v>4</v>
       </c>
       <c r="AD6">
+        <v>4</v>
+      </c>
+      <c r="AE6" t="s">
+        <v>38</v>
+      </c>
+      <c r="AF6">
         <v>178</v>
       </c>
-      <c r="AE6">
-        <v>0</v>
-      </c>
-      <c r="AF6">
-        <v>0</v>
-      </c>
       <c r="AG6">
         <v>0</v>
       </c>
+      <c r="AH6">
+        <v>0</v>
+      </c>
+      <c r="AI6">
+        <v>0</v>
+      </c>
     </row>
-    <row r="7" spans="1:33">
+    <row r="7" spans="1:35">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -1425,23 +1479,29 @@
       <c r="AB7">
         <v>5</v>
       </c>
-      <c r="AC7" t="s">
-        <v>37</v>
+      <c r="AC7">
+        <v>5</v>
       </c>
       <c r="AD7">
+        <v>5</v>
+      </c>
+      <c r="AE7" t="s">
+        <v>39</v>
+      </c>
+      <c r="AF7">
         <v>218</v>
       </c>
-      <c r="AE7">
-        <v>0</v>
-      </c>
-      <c r="AF7">
-        <v>0</v>
-      </c>
       <c r="AG7">
         <v>0</v>
       </c>
+      <c r="AH7">
+        <v>0</v>
+      </c>
+      <c r="AI7">
+        <v>0</v>
+      </c>
     </row>
-    <row r="8" spans="1:33">
+    <row r="8" spans="1:35">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -1526,23 +1586,29 @@
       <c r="AB8">
         <v>6</v>
       </c>
-      <c r="AC8" t="s">
-        <v>38</v>
+      <c r="AC8">
+        <v>6</v>
       </c>
       <c r="AD8">
+        <v>6</v>
+      </c>
+      <c r="AE8" t="s">
+        <v>40</v>
+      </c>
+      <c r="AF8">
         <v>276</v>
       </c>
-      <c r="AE8">
-        <v>0</v>
-      </c>
-      <c r="AF8">
-        <v>0</v>
-      </c>
       <c r="AG8">
         <v>0</v>
       </c>
+      <c r="AH8">
+        <v>0</v>
+      </c>
+      <c r="AI8">
+        <v>0</v>
+      </c>
     </row>
-    <row r="9" spans="1:33">
+    <row r="9" spans="1:35">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -1627,23 +1693,29 @@
       <c r="AB9">
         <v>7</v>
       </c>
-      <c r="AC9" t="s">
-        <v>39</v>
+      <c r="AC9">
+        <v>7</v>
       </c>
       <c r="AD9">
+        <v>7</v>
+      </c>
+      <c r="AE9" t="s">
+        <v>41</v>
+      </c>
+      <c r="AF9">
         <v>321</v>
       </c>
-      <c r="AE9">
-        <v>0</v>
-      </c>
-      <c r="AF9">
-        <v>0</v>
-      </c>
       <c r="AG9">
         <v>0</v>
       </c>
+      <c r="AH9">
+        <v>0</v>
+      </c>
+      <c r="AI9">
+        <v>0</v>
+      </c>
     </row>
-    <row r="10" spans="1:33">
+    <row r="10" spans="1:35">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -1728,23 +1800,29 @@
       <c r="AB10">
         <v>8</v>
       </c>
-      <c r="AC10" t="s">
-        <v>40</v>
+      <c r="AC10">
+        <v>8</v>
       </c>
       <c r="AD10">
+        <v>8</v>
+      </c>
+      <c r="AE10" t="s">
+        <v>42</v>
+      </c>
+      <c r="AF10">
         <v>360</v>
       </c>
-      <c r="AE10">
+      <c r="AG10">
         <v>2</v>
       </c>
-      <c r="AF10">
-        <v>0</v>
-      </c>
-      <c r="AG10">
+      <c r="AH10">
+        <v>0</v>
+      </c>
+      <c r="AI10">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:33">
+    <row r="11" spans="1:35">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -1829,23 +1907,29 @@
       <c r="AB11">
         <v>9</v>
       </c>
-      <c r="AC11" t="s">
-        <v>41</v>
+      <c r="AC11">
+        <v>9</v>
       </c>
       <c r="AD11">
+        <v>9</v>
+      </c>
+      <c r="AE11" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF11">
         <v>396</v>
       </c>
-      <c r="AE11">
+      <c r="AG11">
         <v>2</v>
       </c>
-      <c r="AF11">
-        <v>0</v>
-      </c>
-      <c r="AG11">
+      <c r="AH11">
+        <v>0</v>
+      </c>
+      <c r="AI11">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:33">
+    <row r="12" spans="1:35">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -1930,23 +2014,29 @@
       <c r="AB12">
         <v>10</v>
       </c>
-      <c r="AC12" t="s">
-        <v>42</v>
+      <c r="AC12">
+        <v>10</v>
       </c>
       <c r="AD12">
+        <v>10</v>
+      </c>
+      <c r="AE12" t="s">
+        <v>44</v>
+      </c>
+      <c r="AF12">
         <v>396</v>
       </c>
-      <c r="AE12">
+      <c r="AG12">
         <v>2</v>
       </c>
-      <c r="AF12">
-        <v>0</v>
-      </c>
-      <c r="AG12">
+      <c r="AH12">
+        <v>0</v>
+      </c>
+      <c r="AI12">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:33">
+    <row r="13" spans="1:35">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -2031,23 +2121,29 @@
       <c r="AB13">
         <v>11</v>
       </c>
-      <c r="AC13" t="s">
-        <v>43</v>
+      <c r="AC13">
+        <v>11</v>
       </c>
       <c r="AD13">
+        <v>11</v>
+      </c>
+      <c r="AE13" t="s">
+        <v>45</v>
+      </c>
+      <c r="AF13">
         <v>476</v>
       </c>
-      <c r="AE13">
+      <c r="AG13">
         <v>4</v>
       </c>
-      <c r="AF13">
-        <v>0</v>
-      </c>
-      <c r="AG13">
+      <c r="AH13">
+        <v>0</v>
+      </c>
+      <c r="AI13">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:33">
+    <row r="14" spans="1:35">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -2132,23 +2228,29 @@
       <c r="AB14">
         <v>12</v>
       </c>
-      <c r="AC14" t="s">
-        <v>44</v>
+      <c r="AC14">
+        <v>12</v>
       </c>
       <c r="AD14">
+        <v>12</v>
+      </c>
+      <c r="AE14" t="s">
+        <v>46</v>
+      </c>
+      <c r="AF14">
         <v>541</v>
       </c>
-      <c r="AE14">
+      <c r="AG14">
         <v>4</v>
       </c>
-      <c r="AF14">
-        <v>0</v>
-      </c>
-      <c r="AG14">
+      <c r="AH14">
+        <v>0</v>
+      </c>
+      <c r="AI14">
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:33">
+    <row r="15" spans="1:35">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -2233,23 +2335,29 @@
       <c r="AB15">
         <v>13</v>
       </c>
-      <c r="AC15" t="s">
-        <v>45</v>
+      <c r="AC15">
+        <v>13</v>
       </c>
       <c r="AD15">
+        <v>13</v>
+      </c>
+      <c r="AE15" t="s">
+        <v>47</v>
+      </c>
+      <c r="AF15">
         <v>650</v>
       </c>
-      <c r="AE15">
+      <c r="AG15">
         <v>4</v>
       </c>
-      <c r="AF15">
-        <v>0</v>
-      </c>
-      <c r="AG15">
+      <c r="AH15">
+        <v>0</v>
+      </c>
+      <c r="AI15">
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:33">
+    <row r="16" spans="1:35">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -2334,23 +2442,29 @@
       <c r="AB16">
         <v>14</v>
       </c>
-      <c r="AC16" t="s">
-        <v>46</v>
+      <c r="AC16">
+        <v>14</v>
       </c>
       <c r="AD16">
+        <v>14</v>
+      </c>
+      <c r="AE16" t="s">
+        <v>48</v>
+      </c>
+      <c r="AF16">
         <v>741</v>
       </c>
-      <c r="AE16">
+      <c r="AG16">
         <v>4</v>
       </c>
-      <c r="AF16">
-        <v>0</v>
-      </c>
-      <c r="AG16">
+      <c r="AH16">
+        <v>0</v>
+      </c>
+      <c r="AI16">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:33">
+    <row r="17" spans="1:35">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -2435,23 +2549,29 @@
       <c r="AB17">
         <v>15</v>
       </c>
-      <c r="AC17" t="s">
-        <v>47</v>
+      <c r="AC17">
+        <v>15</v>
       </c>
       <c r="AD17">
+        <v>15</v>
+      </c>
+      <c r="AE17" t="s">
+        <v>49</v>
+      </c>
+      <c r="AF17">
         <v>777</v>
       </c>
-      <c r="AE17">
+      <c r="AG17">
         <v>7</v>
       </c>
-      <c r="AF17">
-        <v>0</v>
-      </c>
-      <c r="AG17">
+      <c r="AH17">
+        <v>0</v>
+      </c>
+      <c r="AI17">
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:33">
+    <row r="18" spans="1:35">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -2536,23 +2656,29 @@
       <c r="AB18">
         <v>16</v>
       </c>
-      <c r="AC18" t="s">
-        <v>48</v>
+      <c r="AC18">
+        <v>16</v>
       </c>
       <c r="AD18">
+        <v>16</v>
+      </c>
+      <c r="AE18" t="s">
+        <v>50</v>
+      </c>
+      <c r="AF18">
         <v>807</v>
       </c>
-      <c r="AE18">
+      <c r="AG18">
         <v>7</v>
       </c>
-      <c r="AF18">
-        <v>0</v>
-      </c>
-      <c r="AG18">
+      <c r="AH18">
+        <v>0</v>
+      </c>
+      <c r="AI18">
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:33">
+    <row r="19" spans="1:35">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -2637,23 +2763,29 @@
       <c r="AB19">
         <v>17</v>
       </c>
-      <c r="AC19" t="s">
-        <v>49</v>
+      <c r="AC19">
+        <v>17</v>
       </c>
       <c r="AD19">
+        <v>17</v>
+      </c>
+      <c r="AE19" t="s">
+        <v>51</v>
+      </c>
+      <c r="AF19">
         <v>858</v>
       </c>
-      <c r="AE19">
+      <c r="AG19">
         <v>7</v>
       </c>
-      <c r="AF19">
-        <v>0</v>
-      </c>
-      <c r="AG19">
+      <c r="AH19">
+        <v>0</v>
+      </c>
+      <c r="AI19">
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:33">
+    <row r="20" spans="1:35">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -2738,23 +2870,29 @@
       <c r="AB20">
         <v>18</v>
       </c>
-      <c r="AC20" t="s">
-        <v>50</v>
+      <c r="AC20">
+        <v>18</v>
       </c>
       <c r="AD20">
+        <v>18</v>
+      </c>
+      <c r="AE20" t="s">
+        <v>52</v>
+      </c>
+      <c r="AF20">
         <v>858</v>
       </c>
-      <c r="AE20">
+      <c r="AG20">
         <v>7</v>
       </c>
-      <c r="AF20">
-        <v>0</v>
-      </c>
-      <c r="AG20">
+      <c r="AH20">
+        <v>0</v>
+      </c>
+      <c r="AI20">
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:33">
+    <row r="21" spans="1:35">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -2839,23 +2977,29 @@
       <c r="AB21">
         <v>19</v>
       </c>
-      <c r="AC21" t="s">
-        <v>51</v>
+      <c r="AC21">
+        <v>19</v>
       </c>
       <c r="AD21">
+        <v>19</v>
+      </c>
+      <c r="AE21" t="s">
+        <v>53</v>
+      </c>
+      <c r="AF21">
         <v>1011</v>
       </c>
-      <c r="AE21">
+      <c r="AG21">
         <v>7</v>
       </c>
-      <c r="AF21">
-        <v>0</v>
-      </c>
-      <c r="AG21">
+      <c r="AH21">
+        <v>0</v>
+      </c>
+      <c r="AI21">
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:33">
+    <row r="22" spans="1:35">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -2940,23 +3084,29 @@
       <c r="AB22">
         <v>20</v>
       </c>
-      <c r="AC22" t="s">
-        <v>52</v>
+      <c r="AC22">
+        <v>20</v>
       </c>
       <c r="AD22">
+        <v>20</v>
+      </c>
+      <c r="AE22" t="s">
+        <v>54</v>
+      </c>
+      <c r="AF22">
         <v>1071</v>
       </c>
-      <c r="AE22">
+      <c r="AG22">
         <v>7</v>
       </c>
-      <c r="AF22">
-        <v>0</v>
-      </c>
-      <c r="AG22">
+      <c r="AH22">
+        <v>0</v>
+      </c>
+      <c r="AI22">
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:33">
+    <row r="23" spans="1:35">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -3041,23 +3191,29 @@
       <c r="AB23">
         <v>21</v>
       </c>
-      <c r="AC23" t="s">
-        <v>53</v>
+      <c r="AC23">
+        <v>21</v>
       </c>
       <c r="AD23">
+        <v>21</v>
+      </c>
+      <c r="AE23" t="s">
+        <v>55</v>
+      </c>
+      <c r="AF23">
         <v>1126</v>
       </c>
-      <c r="AE23">
+      <c r="AG23">
         <v>7</v>
       </c>
-      <c r="AF23">
-        <v>0</v>
-      </c>
-      <c r="AG23">
+      <c r="AH23">
+        <v>0</v>
+      </c>
+      <c r="AI23">
         <v>1119</v>
       </c>
     </row>
-    <row r="24" spans="1:33">
+    <row r="24" spans="1:35">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -3142,23 +3298,29 @@
       <c r="AB24">
         <v>22</v>
       </c>
-      <c r="AC24" t="s">
-        <v>54</v>
+      <c r="AC24">
+        <v>22</v>
       </c>
       <c r="AD24">
+        <v>22</v>
+      </c>
+      <c r="AE24" t="s">
+        <v>56</v>
+      </c>
+      <c r="AF24">
         <v>1157</v>
       </c>
-      <c r="AE24">
+      <c r="AG24">
         <v>7</v>
       </c>
-      <c r="AF24">
-        <v>0</v>
-      </c>
-      <c r="AG24">
+      <c r="AH24">
+        <v>0</v>
+      </c>
+      <c r="AI24">
         <v>1150</v>
       </c>
     </row>
-    <row r="25" spans="1:33">
+    <row r="25" spans="1:35">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -3243,23 +3405,29 @@
       <c r="AB25">
         <v>23</v>
       </c>
-      <c r="AC25" t="s">
-        <v>55</v>
+      <c r="AC25">
+        <v>23</v>
       </c>
       <c r="AD25">
+        <v>23</v>
+      </c>
+      <c r="AE25" t="s">
+        <v>57</v>
+      </c>
+      <c r="AF25">
         <v>1187</v>
       </c>
-      <c r="AE25">
+      <c r="AG25">
         <v>7</v>
       </c>
-      <c r="AF25">
-        <v>0</v>
-      </c>
-      <c r="AG25">
+      <c r="AH25">
+        <v>0</v>
+      </c>
+      <c r="AI25">
         <v>1180</v>
       </c>
     </row>
-    <row r="26" spans="1:33">
+    <row r="26" spans="1:35">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -3344,23 +3512,29 @@
       <c r="AB26">
         <v>24</v>
       </c>
-      <c r="AC26" t="s">
-        <v>56</v>
+      <c r="AC26">
+        <v>24</v>
       </c>
       <c r="AD26">
+        <v>24</v>
+      </c>
+      <c r="AE26" t="s">
+        <v>58</v>
+      </c>
+      <c r="AF26">
         <v>1285</v>
       </c>
-      <c r="AE26">
+      <c r="AG26">
         <v>7</v>
       </c>
-      <c r="AF26">
-        <v>0</v>
-      </c>
-      <c r="AG26">
+      <c r="AH26">
+        <v>0</v>
+      </c>
+      <c r="AI26">
         <v>1278</v>
       </c>
     </row>
-    <row r="27" spans="1:33">
+    <row r="27" spans="1:35">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -3445,23 +3619,29 @@
       <c r="AB27">
         <v>25</v>
       </c>
-      <c r="AC27" t="s">
-        <v>57</v>
+      <c r="AC27">
+        <v>25</v>
       </c>
       <c r="AD27">
+        <v>25</v>
+      </c>
+      <c r="AE27" t="s">
+        <v>59</v>
+      </c>
+      <c r="AF27">
         <v>1377</v>
       </c>
-      <c r="AE27">
+      <c r="AG27">
         <v>7</v>
       </c>
-      <c r="AF27">
-        <v>0</v>
-      </c>
-      <c r="AG27">
+      <c r="AH27">
+        <v>0</v>
+      </c>
+      <c r="AI27">
         <v>1370</v>
       </c>
     </row>
-    <row r="28" spans="1:33">
+    <row r="28" spans="1:35">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -3546,23 +3726,29 @@
       <c r="AB28">
         <v>26</v>
       </c>
-      <c r="AC28" t="s">
-        <v>58</v>
+      <c r="AC28">
+        <v>26</v>
       </c>
       <c r="AD28">
+        <v>26</v>
+      </c>
+      <c r="AE28" t="s">
+        <v>60</v>
+      </c>
+      <c r="AF28">
         <v>1456</v>
       </c>
-      <c r="AE28">
+      <c r="AG28">
         <v>12</v>
       </c>
-      <c r="AF28">
-        <v>0</v>
-      </c>
-      <c r="AG28">
+      <c r="AH28">
+        <v>0</v>
+      </c>
+      <c r="AI28">
         <v>1444</v>
       </c>
     </row>
-    <row r="29" spans="1:33">
+    <row r="29" spans="1:35">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -3647,23 +3833,29 @@
       <c r="AB29">
         <v>27</v>
       </c>
-      <c r="AC29" t="s">
-        <v>59</v>
+      <c r="AC29">
+        <v>27</v>
       </c>
       <c r="AD29">
+        <v>27</v>
+      </c>
+      <c r="AE29" t="s">
+        <v>61</v>
+      </c>
+      <c r="AF29">
         <v>1547</v>
       </c>
-      <c r="AE29">
+      <c r="AG29">
         <v>13</v>
       </c>
-      <c r="AF29">
-        <v>0</v>
-      </c>
-      <c r="AG29">
+      <c r="AH29">
+        <v>0</v>
+      </c>
+      <c r="AI29">
         <v>1534</v>
       </c>
     </row>
-    <row r="30" spans="1:33">
+    <row r="30" spans="1:35">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -3748,23 +3940,29 @@
       <c r="AB30">
         <v>28</v>
       </c>
-      <c r="AC30" t="s">
-        <v>60</v>
+      <c r="AC30">
+        <v>28</v>
       </c>
       <c r="AD30">
+        <v>28</v>
+      </c>
+      <c r="AE30" t="s">
+        <v>62</v>
+      </c>
+      <c r="AF30">
         <v>1615</v>
       </c>
-      <c r="AE30">
+      <c r="AG30">
         <v>15</v>
       </c>
-      <c r="AF30">
-        <v>0</v>
-      </c>
-      <c r="AG30">
+      <c r="AH30">
+        <v>0</v>
+      </c>
+      <c r="AI30">
         <v>1600</v>
       </c>
     </row>
-    <row r="31" spans="1:33">
+    <row r="31" spans="1:35">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -3849,23 +4047,29 @@
       <c r="AB31">
         <v>29</v>
       </c>
-      <c r="AC31" t="s">
-        <v>61</v>
+      <c r="AC31">
+        <v>29</v>
       </c>
       <c r="AD31">
+        <v>29</v>
+      </c>
+      <c r="AE31" t="s">
+        <v>63</v>
+      </c>
+      <c r="AF31">
         <v>1671</v>
       </c>
-      <c r="AE31">
+      <c r="AG31">
         <v>15</v>
       </c>
-      <c r="AF31">
-        <v>0</v>
-      </c>
-      <c r="AG31">
+      <c r="AH31">
+        <v>0</v>
+      </c>
+      <c r="AI31">
         <v>1656</v>
       </c>
     </row>
-    <row r="32" spans="1:33">
+    <row r="32" spans="1:35">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -3950,23 +4154,29 @@
       <c r="AB32">
         <v>30</v>
       </c>
-      <c r="AC32" t="s">
-        <v>62</v>
+      <c r="AC32">
+        <v>30</v>
       </c>
       <c r="AD32">
+        <v>30</v>
+      </c>
+      <c r="AE32" t="s">
+        <v>64</v>
+      </c>
+      <c r="AF32">
         <v>1714</v>
       </c>
-      <c r="AE32">
+      <c r="AG32">
         <v>18</v>
       </c>
-      <c r="AF32">
-        <v>0</v>
-      </c>
-      <c r="AG32">
+      <c r="AH32">
+        <v>0</v>
+      </c>
+      <c r="AI32">
         <v>1696</v>
       </c>
     </row>
-    <row r="33" spans="1:33">
+    <row r="33" spans="1:35">
       <c r="A33" s="1">
         <v>31</v>
       </c>
@@ -4051,23 +4261,29 @@
       <c r="AB33">
         <v>31</v>
       </c>
-      <c r="AC33" t="s">
-        <v>63</v>
+      <c r="AC33">
+        <v>31</v>
       </c>
       <c r="AD33">
+        <v>31</v>
+      </c>
+      <c r="AE33" t="s">
+        <v>65</v>
+      </c>
+      <c r="AF33">
         <v>1795</v>
       </c>
-      <c r="AE33">
+      <c r="AG33">
         <v>18</v>
       </c>
-      <c r="AF33">
-        <v>0</v>
-      </c>
-      <c r="AG33">
+      <c r="AH33">
+        <v>0</v>
+      </c>
+      <c r="AI33">
         <v>1777</v>
       </c>
     </row>
-    <row r="34" spans="1:33">
+    <row r="34" spans="1:35">
       <c r="A34" s="1">
         <v>32</v>
       </c>
@@ -4152,23 +4368,29 @@
       <c r="AB34">
         <v>32</v>
       </c>
-      <c r="AC34" t="s">
-        <v>64</v>
+      <c r="AC34">
+        <v>32</v>
       </c>
       <c r="AD34">
+        <v>32</v>
+      </c>
+      <c r="AE34" t="s">
+        <v>66</v>
+      </c>
+      <c r="AF34">
         <v>1889</v>
       </c>
-      <c r="AE34">
+      <c r="AG34">
         <v>20</v>
       </c>
-      <c r="AF34">
-        <v>0</v>
-      </c>
-      <c r="AG34">
+      <c r="AH34">
+        <v>0</v>
+      </c>
+      <c r="AI34">
         <v>1869</v>
       </c>
     </row>
-    <row r="35" spans="1:33">
+    <row r="35" spans="1:35">
       <c r="A35" s="1">
         <v>33</v>
       </c>
@@ -4253,23 +4475,29 @@
       <c r="AB35">
         <v>33</v>
       </c>
-      <c r="AC35" t="s">
-        <v>65</v>
+      <c r="AC35">
+        <v>33</v>
       </c>
       <c r="AD35">
+        <v>33</v>
+      </c>
+      <c r="AE35" t="s">
+        <v>67</v>
+      </c>
+      <c r="AF35">
         <v>1975</v>
       </c>
-      <c r="AE35">
+      <c r="AG35">
         <v>23</v>
       </c>
-      <c r="AF35">
-        <v>0</v>
-      </c>
-      <c r="AG35">
+      <c r="AH35">
+        <v>0</v>
+      </c>
+      <c r="AI35">
         <v>1952</v>
       </c>
     </row>
-    <row r="36" spans="1:33">
+    <row r="36" spans="1:35">
       <c r="A36" s="1">
         <v>34</v>
       </c>
@@ -4354,23 +4582,29 @@
       <c r="AB36">
         <v>34</v>
       </c>
-      <c r="AC36" t="s">
-        <v>66</v>
+      <c r="AC36">
+        <v>34</v>
       </c>
       <c r="AD36">
+        <v>34</v>
+      </c>
+      <c r="AE36" t="s">
+        <v>68</v>
+      </c>
+      <c r="AF36">
         <v>2051</v>
       </c>
-      <c r="AE36">
+      <c r="AG36">
         <v>24</v>
       </c>
-      <c r="AF36">
-        <v>0</v>
-      </c>
-      <c r="AG36">
+      <c r="AH36">
+        <v>0</v>
+      </c>
+      <c r="AI36">
         <v>2027</v>
       </c>
     </row>
-    <row r="37" spans="1:33">
+    <row r="37" spans="1:35">
       <c r="A37" s="1">
         <v>35</v>
       </c>
@@ -4455,23 +4689,29 @@
       <c r="AB37">
         <v>35</v>
       </c>
-      <c r="AC37" t="s">
-        <v>67</v>
+      <c r="AC37">
+        <v>35</v>
       </c>
       <c r="AD37">
+        <v>35</v>
+      </c>
+      <c r="AE37" t="s">
+        <v>69</v>
+      </c>
+      <c r="AF37">
         <v>2144</v>
       </c>
-      <c r="AE37">
+      <c r="AG37">
         <v>24</v>
       </c>
-      <c r="AF37">
-        <v>0</v>
-      </c>
-      <c r="AG37">
+      <c r="AH37">
+        <v>0</v>
+      </c>
+      <c r="AI37">
         <v>2120</v>
       </c>
     </row>
-    <row r="38" spans="1:33">
+    <row r="38" spans="1:35">
       <c r="A38" s="1">
         <v>36</v>
       </c>
@@ -4556,23 +4796,29 @@
       <c r="AB38">
         <v>36</v>
       </c>
-      <c r="AC38" t="s">
-        <v>68</v>
+      <c r="AC38">
+        <v>36</v>
       </c>
       <c r="AD38">
+        <v>36</v>
+      </c>
+      <c r="AE38" t="s">
+        <v>70</v>
+      </c>
+      <c r="AF38">
         <v>2190</v>
       </c>
-      <c r="AE38">
+      <c r="AG38">
         <v>24</v>
       </c>
-      <c r="AF38">
-        <v>0</v>
-      </c>
-      <c r="AG38">
+      <c r="AH38">
+        <v>0</v>
+      </c>
+      <c r="AI38">
         <v>2166</v>
       </c>
     </row>
-    <row r="39" spans="1:33">
+    <row r="39" spans="1:35">
       <c r="A39" s="1">
         <v>37</v>
       </c>
@@ -4657,23 +4903,29 @@
       <c r="AB39">
         <v>37</v>
       </c>
-      <c r="AC39" t="s">
-        <v>69</v>
+      <c r="AC39">
+        <v>37</v>
       </c>
       <c r="AD39">
+        <v>37</v>
+      </c>
+      <c r="AE39" t="s">
+        <v>71</v>
+      </c>
+      <c r="AF39">
         <v>2256</v>
       </c>
-      <c r="AE39">
+      <c r="AG39">
         <v>24</v>
       </c>
-      <c r="AF39">
-        <v>0</v>
-      </c>
-      <c r="AG39">
+      <c r="AH39">
+        <v>0</v>
+      </c>
+      <c r="AI39">
         <v>2232</v>
       </c>
     </row>
-    <row r="40" spans="1:33">
+    <row r="40" spans="1:35">
       <c r="A40" s="1">
         <v>38</v>
       </c>
@@ -4758,23 +5010,29 @@
       <c r="AB40">
         <v>38</v>
       </c>
-      <c r="AC40" t="s">
-        <v>70</v>
+      <c r="AC40">
+        <v>38</v>
       </c>
       <c r="AD40">
+        <v>38</v>
+      </c>
+      <c r="AE40" t="s">
+        <v>72</v>
+      </c>
+      <c r="AF40">
         <v>2348</v>
       </c>
-      <c r="AE40">
+      <c r="AG40">
         <v>28</v>
       </c>
-      <c r="AF40">
-        <v>0</v>
-      </c>
-      <c r="AG40">
+      <c r="AH40">
+        <v>0</v>
+      </c>
+      <c r="AI40">
         <v>2320</v>
       </c>
     </row>
-    <row r="41" spans="1:33">
+    <row r="41" spans="1:35">
       <c r="A41" s="1">
         <v>39</v>
       </c>
@@ -4859,23 +5117,29 @@
       <c r="AB41">
         <v>39</v>
       </c>
-      <c r="AC41" t="s">
-        <v>71</v>
+      <c r="AC41">
+        <v>39</v>
       </c>
       <c r="AD41">
+        <v>39</v>
+      </c>
+      <c r="AE41" t="s">
+        <v>73</v>
+      </c>
+      <c r="AF41">
         <v>2438</v>
       </c>
-      <c r="AE41">
+      <c r="AG41">
         <v>29</v>
       </c>
-      <c r="AF41">
-        <v>0</v>
-      </c>
-      <c r="AG41">
+      <c r="AH41">
+        <v>0</v>
+      </c>
+      <c r="AI41">
         <v>2409</v>
       </c>
     </row>
-    <row r="42" spans="1:33">
+    <row r="42" spans="1:35">
       <c r="A42" s="1">
         <v>40</v>
       </c>
@@ -4960,23 +5224,29 @@
       <c r="AB42">
         <v>40</v>
       </c>
-      <c r="AC42" t="s">
-        <v>72</v>
+      <c r="AC42">
+        <v>40</v>
       </c>
       <c r="AD42">
+        <v>40</v>
+      </c>
+      <c r="AE42" t="s">
+        <v>74</v>
+      </c>
+      <c r="AF42">
         <v>2526</v>
       </c>
-      <c r="AE42">
+      <c r="AG42">
         <v>29</v>
       </c>
-      <c r="AF42">
-        <v>0</v>
-      </c>
-      <c r="AG42">
+      <c r="AH42">
+        <v>0</v>
+      </c>
+      <c r="AI42">
         <v>2497</v>
       </c>
     </row>
-    <row r="43" spans="1:33">
+    <row r="43" spans="1:35">
       <c r="A43" s="1">
         <v>41</v>
       </c>
@@ -5061,23 +5331,29 @@
       <c r="AB43">
         <v>41</v>
       </c>
-      <c r="AC43" t="s">
-        <v>73</v>
+      <c r="AC43">
+        <v>41</v>
       </c>
       <c r="AD43">
+        <v>41</v>
+      </c>
+      <c r="AE43" t="s">
+        <v>75</v>
+      </c>
+      <c r="AF43">
         <v>2609</v>
       </c>
-      <c r="AE43">
+      <c r="AG43">
         <v>30</v>
       </c>
-      <c r="AF43">
-        <v>0</v>
-      </c>
-      <c r="AG43">
+      <c r="AH43">
+        <v>0</v>
+      </c>
+      <c r="AI43">
         <v>2579</v>
       </c>
     </row>
-    <row r="44" spans="1:33">
+    <row r="44" spans="1:35">
       <c r="A44" s="1">
         <v>42</v>
       </c>
@@ -5162,23 +5438,29 @@
       <c r="AB44">
         <v>42</v>
       </c>
-      <c r="AC44" t="s">
-        <v>74</v>
+      <c r="AC44">
+        <v>42</v>
       </c>
       <c r="AD44">
+        <v>42</v>
+      </c>
+      <c r="AE44" t="s">
+        <v>76</v>
+      </c>
+      <c r="AF44">
         <v>2707</v>
       </c>
-      <c r="AE44">
+      <c r="AG44">
         <v>31</v>
       </c>
-      <c r="AF44">
-        <v>0</v>
-      </c>
-      <c r="AG44">
+      <c r="AH44">
+        <v>0</v>
+      </c>
+      <c r="AI44">
         <v>2676</v>
       </c>
     </row>
-    <row r="45" spans="1:33">
+    <row r="45" spans="1:35">
       <c r="A45" s="1">
         <v>43</v>
       </c>
@@ -5263,23 +5545,29 @@
       <c r="AB45">
         <v>43</v>
       </c>
-      <c r="AC45" t="s">
-        <v>75</v>
+      <c r="AC45">
+        <v>43</v>
       </c>
       <c r="AD45">
+        <v>43</v>
+      </c>
+      <c r="AE45" t="s">
+        <v>77</v>
+      </c>
+      <c r="AF45">
         <v>2769</v>
       </c>
-      <c r="AE45">
+      <c r="AG45">
         <v>31</v>
       </c>
-      <c r="AF45">
-        <v>0</v>
-      </c>
-      <c r="AG45">
+      <c r="AH45">
+        <v>0</v>
+      </c>
+      <c r="AI45">
         <v>2738</v>
       </c>
     </row>
-    <row r="46" spans="1:33">
+    <row r="46" spans="1:35">
       <c r="A46" s="1">
         <v>44</v>
       </c>
@@ -5364,23 +5652,29 @@
       <c r="AB46">
         <v>44</v>
       </c>
-      <c r="AC46" t="s">
-        <v>76</v>
+      <c r="AC46">
+        <v>44</v>
       </c>
       <c r="AD46">
+        <v>44</v>
+      </c>
+      <c r="AE46" t="s">
+        <v>78</v>
+      </c>
+      <c r="AF46">
         <v>2832</v>
       </c>
-      <c r="AE46">
+      <c r="AG46">
         <v>35</v>
       </c>
-      <c r="AF46">
-        <v>0</v>
-      </c>
-      <c r="AG46">
+      <c r="AH46">
+        <v>0</v>
+      </c>
+      <c r="AI46">
         <v>2797</v>
       </c>
     </row>
-    <row r="47" spans="1:33">
+    <row r="47" spans="1:35">
       <c r="A47" s="1">
         <v>45</v>
       </c>
@@ -5465,23 +5759,29 @@
       <c r="AB47">
         <v>45</v>
       </c>
-      <c r="AC47" t="s">
-        <v>77</v>
+      <c r="AC47">
+        <v>45</v>
       </c>
       <c r="AD47">
+        <v>45</v>
+      </c>
+      <c r="AE47" t="s">
+        <v>79</v>
+      </c>
+      <c r="AF47">
         <v>2912</v>
       </c>
-      <c r="AE47">
+      <c r="AG47">
         <v>37</v>
       </c>
-      <c r="AF47">
-        <v>0</v>
-      </c>
-      <c r="AG47">
+      <c r="AH47">
+        <v>0</v>
+      </c>
+      <c r="AI47">
         <v>2875</v>
       </c>
     </row>
-    <row r="48" spans="1:33">
+    <row r="48" spans="1:35">
       <c r="A48" s="1">
         <v>46</v>
       </c>
@@ -5566,23 +5866,29 @@
       <c r="AB48">
         <v>46</v>
       </c>
-      <c r="AC48" t="s">
-        <v>78</v>
+      <c r="AC48">
+        <v>46</v>
       </c>
       <c r="AD48">
+        <v>46</v>
+      </c>
+      <c r="AE48" t="s">
+        <v>80</v>
+      </c>
+      <c r="AF48">
         <v>3010</v>
       </c>
-      <c r="AE48">
+      <c r="AG48">
         <v>39</v>
       </c>
-      <c r="AF48">
-        <v>0</v>
-      </c>
-      <c r="AG48">
+      <c r="AH48">
+        <v>0</v>
+      </c>
+      <c r="AI48">
         <v>2971</v>
       </c>
     </row>
-    <row r="49" spans="1:33">
+    <row r="49" spans="1:35">
       <c r="A49" s="1">
         <v>47</v>
       </c>
@@ -5667,23 +5973,29 @@
       <c r="AB49">
         <v>47</v>
       </c>
-      <c r="AC49" t="s">
-        <v>79</v>
+      <c r="AC49">
+        <v>47</v>
       </c>
       <c r="AD49">
+        <v>47</v>
+      </c>
+      <c r="AE49" t="s">
+        <v>81</v>
+      </c>
+      <c r="AF49">
         <v>3104</v>
       </c>
-      <c r="AE49">
+      <c r="AG49">
         <v>39</v>
       </c>
-      <c r="AF49">
-        <v>0</v>
-      </c>
-      <c r="AG49">
+      <c r="AH49">
+        <v>0</v>
+      </c>
+      <c r="AI49">
         <v>3065</v>
       </c>
     </row>
-    <row r="50" spans="1:33">
+    <row r="50" spans="1:35">
       <c r="A50" s="1">
         <v>48</v>
       </c>
@@ -5768,23 +6080,29 @@
       <c r="AB50">
         <v>48</v>
       </c>
-      <c r="AC50" t="s">
-        <v>80</v>
+      <c r="AC50">
+        <v>48</v>
       </c>
       <c r="AD50">
+        <v>48</v>
+      </c>
+      <c r="AE50" t="s">
+        <v>82</v>
+      </c>
+      <c r="AF50">
         <v>3206</v>
       </c>
-      <c r="AE50">
+      <c r="AG50">
         <v>43</v>
       </c>
-      <c r="AF50">
-        <v>0</v>
-      </c>
-      <c r="AG50">
+      <c r="AH50">
+        <v>0</v>
+      </c>
+      <c r="AI50">
         <v>3163</v>
       </c>
     </row>
-    <row r="51" spans="1:33">
+    <row r="51" spans="1:35">
       <c r="A51" s="1">
         <v>49</v>
       </c>
@@ -5869,23 +6187,29 @@
       <c r="AB51">
         <v>49</v>
       </c>
-      <c r="AC51" t="s">
-        <v>81</v>
+      <c r="AC51">
+        <v>49</v>
       </c>
       <c r="AD51">
+        <v>49</v>
+      </c>
+      <c r="AE51" t="s">
+        <v>83</v>
+      </c>
+      <c r="AF51">
         <v>3291</v>
       </c>
-      <c r="AE51">
+      <c r="AG51">
         <v>44</v>
       </c>
-      <c r="AF51">
-        <v>0</v>
-      </c>
-      <c r="AG51">
+      <c r="AH51">
+        <v>0</v>
+      </c>
+      <c r="AI51">
         <v>3247</v>
       </c>
     </row>
-    <row r="52" spans="1:33">
+    <row r="52" spans="1:35">
       <c r="A52" s="1">
         <v>50</v>
       </c>
@@ -5970,23 +6294,29 @@
       <c r="AB52">
         <v>50</v>
       </c>
-      <c r="AC52" t="s">
-        <v>82</v>
+      <c r="AC52">
+        <v>50</v>
       </c>
       <c r="AD52">
+        <v>50</v>
+      </c>
+      <c r="AE52" t="s">
+        <v>84</v>
+      </c>
+      <c r="AF52">
         <v>3365</v>
       </c>
-      <c r="AE52">
+      <c r="AG52">
         <v>45</v>
       </c>
-      <c r="AF52">
-        <v>0</v>
-      </c>
-      <c r="AG52">
+      <c r="AH52">
+        <v>0</v>
+      </c>
+      <c r="AI52">
         <v>3320</v>
       </c>
     </row>
-    <row r="53" spans="1:33">
+    <row r="53" spans="1:35">
       <c r="A53" s="1">
         <v>51</v>
       </c>
@@ -6071,23 +6401,29 @@
       <c r="AB53">
         <v>51</v>
       </c>
-      <c r="AC53" t="s">
-        <v>83</v>
+      <c r="AC53">
+        <v>51</v>
       </c>
       <c r="AD53">
+        <v>51</v>
+      </c>
+      <c r="AE53" t="s">
+        <v>85</v>
+      </c>
+      <c r="AF53">
         <v>3414</v>
       </c>
-      <c r="AE53">
+      <c r="AG53">
         <v>49</v>
       </c>
-      <c r="AF53">
-        <v>0</v>
-      </c>
-      <c r="AG53">
+      <c r="AH53">
+        <v>0</v>
+      </c>
+      <c r="AI53">
         <v>3365</v>
       </c>
     </row>
-    <row r="54" spans="1:33">
+    <row r="54" spans="1:35">
       <c r="A54" s="1">
         <v>52</v>
       </c>
@@ -6172,23 +6508,29 @@
       <c r="AB54">
         <v>52</v>
       </c>
-      <c r="AC54" t="s">
-        <v>84</v>
+      <c r="AC54">
+        <v>52</v>
       </c>
       <c r="AD54">
+        <v>52</v>
+      </c>
+      <c r="AE54" t="s">
+        <v>86</v>
+      </c>
+      <c r="AF54">
         <v>3530</v>
       </c>
-      <c r="AE54">
+      <c r="AG54">
         <v>51</v>
       </c>
-      <c r="AF54">
-        <v>0</v>
-      </c>
-      <c r="AG54">
+      <c r="AH54">
+        <v>0</v>
+      </c>
+      <c r="AI54">
         <v>3479</v>
       </c>
     </row>
-    <row r="55" spans="1:33">
+    <row r="55" spans="1:35">
       <c r="A55" s="1">
         <v>53</v>
       </c>
@@ -6273,23 +6615,29 @@
       <c r="AB55">
         <v>53</v>
       </c>
-      <c r="AC55" t="s">
-        <v>85</v>
+      <c r="AC55">
+        <v>53</v>
       </c>
       <c r="AD55">
+        <v>53</v>
+      </c>
+      <c r="AE55" t="s">
+        <v>87</v>
+      </c>
+      <c r="AF55">
         <v>3604</v>
       </c>
-      <c r="AE55">
+      <c r="AG55">
         <v>51</v>
       </c>
-      <c r="AF55">
-        <v>0</v>
-      </c>
-      <c r="AG55">
+      <c r="AH55">
+        <v>0</v>
+      </c>
+      <c r="AI55">
         <v>3553</v>
       </c>
     </row>
-    <row r="56" spans="1:33">
+    <row r="56" spans="1:35">
       <c r="A56" s="1">
         <v>54</v>
       </c>
@@ -6374,23 +6722,29 @@
       <c r="AB56">
         <v>54</v>
       </c>
-      <c r="AC56" t="s">
-        <v>86</v>
+      <c r="AC56">
+        <v>54</v>
       </c>
       <c r="AD56">
+        <v>54</v>
+      </c>
+      <c r="AE56" t="s">
+        <v>88</v>
+      </c>
+      <c r="AF56">
         <v>3709</v>
       </c>
-      <c r="AE56">
+      <c r="AG56">
         <v>52</v>
       </c>
-      <c r="AF56">
-        <v>0</v>
-      </c>
-      <c r="AG56">
+      <c r="AH56">
+        <v>0</v>
+      </c>
+      <c r="AI56">
         <v>3657</v>
       </c>
     </row>
-    <row r="57" spans="1:33">
+    <row r="57" spans="1:35">
       <c r="A57" s="1">
         <v>55</v>
       </c>
@@ -6475,23 +6829,29 @@
       <c r="AB57">
         <v>55</v>
       </c>
-      <c r="AC57" t="s">
-        <v>87</v>
+      <c r="AC57">
+        <v>55</v>
       </c>
       <c r="AD57">
+        <v>55</v>
+      </c>
+      <c r="AE57" t="s">
+        <v>89</v>
+      </c>
+      <c r="AF57">
         <v>3785</v>
       </c>
-      <c r="AE57">
+      <c r="AG57">
         <v>53</v>
       </c>
-      <c r="AF57">
-        <v>0</v>
-      </c>
-      <c r="AG57">
+      <c r="AH57">
+        <v>0</v>
+      </c>
+      <c r="AI57">
         <v>3732</v>
       </c>
     </row>
-    <row r="58" spans="1:33">
+    <row r="58" spans="1:35">
       <c r="A58" s="1">
         <v>56</v>
       </c>
@@ -6576,23 +6936,29 @@
       <c r="AB58">
         <v>56</v>
       </c>
-      <c r="AC58" t="s">
-        <v>88</v>
+      <c r="AC58">
+        <v>56</v>
       </c>
       <c r="AD58">
+        <v>56</v>
+      </c>
+      <c r="AE58" t="s">
+        <v>90</v>
+      </c>
+      <c r="AF58">
         <v>3883</v>
       </c>
-      <c r="AE58">
+      <c r="AG58">
         <v>55</v>
       </c>
-      <c r="AF58">
-        <v>0</v>
-      </c>
-      <c r="AG58">
+      <c r="AH58">
+        <v>0</v>
+      </c>
+      <c r="AI58">
         <v>3828</v>
       </c>
     </row>
-    <row r="59" spans="1:33">
+    <row r="59" spans="1:35">
       <c r="A59" s="1">
         <v>57</v>
       </c>
@@ -6677,23 +7043,29 @@
       <c r="AB59">
         <v>57</v>
       </c>
-      <c r="AC59" t="s">
-        <v>89</v>
+      <c r="AC59">
+        <v>57</v>
       </c>
       <c r="AD59">
+        <v>57</v>
+      </c>
+      <c r="AE59" t="s">
+        <v>91</v>
+      </c>
+      <c r="AF59">
         <v>3942</v>
       </c>
-      <c r="AE59">
+      <c r="AG59">
         <v>55</v>
       </c>
-      <c r="AF59">
-        <v>0</v>
-      </c>
-      <c r="AG59">
+      <c r="AH59">
+        <v>0</v>
+      </c>
+      <c r="AI59">
         <v>3887</v>
       </c>
     </row>
-    <row r="60" spans="1:33">
+    <row r="60" spans="1:35">
       <c r="A60" s="1">
         <v>58</v>
       </c>
@@ -6778,23 +7150,29 @@
       <c r="AB60">
         <v>58</v>
       </c>
-      <c r="AC60" t="s">
-        <v>90</v>
+      <c r="AC60">
+        <v>58</v>
       </c>
       <c r="AD60">
+        <v>58</v>
+      </c>
+      <c r="AE60" t="s">
+        <v>92</v>
+      </c>
+      <c r="AF60">
         <v>4019</v>
       </c>
-      <c r="AE60">
+      <c r="AG60">
         <v>61</v>
       </c>
-      <c r="AF60">
-        <v>0</v>
-      </c>
-      <c r="AG60">
+      <c r="AH60">
+        <v>0</v>
+      </c>
+      <c r="AI60">
         <v>3958</v>
       </c>
     </row>
-    <row r="61" spans="1:33">
+    <row r="61" spans="1:35">
       <c r="A61" s="1">
         <v>59</v>
       </c>
@@ -6879,23 +7257,29 @@
       <c r="AB61">
         <v>59</v>
       </c>
-      <c r="AC61" t="s">
-        <v>91</v>
+      <c r="AC61">
+        <v>59</v>
       </c>
       <c r="AD61">
+        <v>59</v>
+      </c>
+      <c r="AE61" t="s">
+        <v>93</v>
+      </c>
+      <c r="AF61">
         <v>4123</v>
       </c>
-      <c r="AE61">
+      <c r="AG61">
         <v>62</v>
       </c>
-      <c r="AF61">
-        <v>0</v>
-      </c>
-      <c r="AG61">
+      <c r="AH61">
+        <v>0</v>
+      </c>
+      <c r="AI61">
         <v>4061</v>
       </c>
     </row>
-    <row r="62" spans="1:33">
+    <row r="62" spans="1:35">
       <c r="A62" s="1">
         <v>60</v>
       </c>
@@ -6980,23 +7364,29 @@
       <c r="AB62">
         <v>60</v>
       </c>
-      <c r="AC62" t="s">
-        <v>92</v>
+      <c r="AC62">
+        <v>60</v>
       </c>
       <c r="AD62">
+        <v>60</v>
+      </c>
+      <c r="AE62" t="s">
+        <v>94</v>
+      </c>
+      <c r="AF62">
         <v>4217</v>
       </c>
-      <c r="AE62">
+      <c r="AG62">
         <v>64</v>
       </c>
-      <c r="AF62">
-        <v>0</v>
-      </c>
-      <c r="AG62">
+      <c r="AH62">
+        <v>0</v>
+      </c>
+      <c r="AI62">
         <v>4153</v>
       </c>
     </row>
-    <row r="63" spans="1:33">
+    <row r="63" spans="1:35">
       <c r="A63" s="1">
         <v>61</v>
       </c>
@@ -7081,23 +7471,29 @@
       <c r="AB63">
         <v>61</v>
       </c>
-      <c r="AC63" t="s">
-        <v>93</v>
+      <c r="AC63">
+        <v>61</v>
       </c>
       <c r="AD63">
+        <v>61</v>
+      </c>
+      <c r="AE63" t="s">
+        <v>95</v>
+      </c>
+      <c r="AF63">
         <v>4308</v>
       </c>
-      <c r="AE63">
+      <c r="AG63">
         <v>64</v>
       </c>
-      <c r="AF63">
-        <v>0</v>
-      </c>
-      <c r="AG63">
+      <c r="AH63">
+        <v>0</v>
+      </c>
+      <c r="AI63">
         <v>4244</v>
       </c>
     </row>
-    <row r="64" spans="1:33">
+    <row r="64" spans="1:35">
       <c r="A64" s="1">
         <v>62</v>
       </c>
@@ -7182,23 +7578,29 @@
       <c r="AB64">
         <v>62</v>
       </c>
-      <c r="AC64" t="s">
-        <v>94</v>
+      <c r="AC64">
+        <v>62</v>
       </c>
       <c r="AD64">
+        <v>62</v>
+      </c>
+      <c r="AE64" t="s">
+        <v>96</v>
+      </c>
+      <c r="AF64">
         <v>4441</v>
       </c>
-      <c r="AE64">
+      <c r="AG64">
         <v>67</v>
       </c>
-      <c r="AF64">
-        <v>0</v>
-      </c>
-      <c r="AG64">
+      <c r="AH64">
+        <v>0</v>
+      </c>
+      <c r="AI64">
         <v>4374</v>
       </c>
     </row>
-    <row r="65" spans="1:33">
+    <row r="65" spans="1:35">
       <c r="A65" s="1">
         <v>63</v>
       </c>
@@ -7283,23 +7685,29 @@
       <c r="AB65">
         <v>63</v>
       </c>
-      <c r="AC65" t="s">
-        <v>95</v>
+      <c r="AC65">
+        <v>63</v>
       </c>
       <c r="AD65">
+        <v>63</v>
+      </c>
+      <c r="AE65" t="s">
+        <v>97</v>
+      </c>
+      <c r="AF65">
         <v>4515</v>
       </c>
-      <c r="AE65">
+      <c r="AG65">
         <v>67</v>
       </c>
-      <c r="AF65">
-        <v>0</v>
-      </c>
-      <c r="AG65">
+      <c r="AH65">
+        <v>0</v>
+      </c>
+      <c r="AI65">
         <v>4448</v>
       </c>
     </row>
-    <row r="66" spans="1:33">
+    <row r="66" spans="1:35">
       <c r="A66" s="1">
         <v>64</v>
       </c>
@@ -7384,23 +7792,29 @@
       <c r="AB66">
         <v>64</v>
       </c>
-      <c r="AC66" t="s">
-        <v>96</v>
+      <c r="AC66">
+        <v>64</v>
       </c>
       <c r="AD66">
+        <v>64</v>
+      </c>
+      <c r="AE66" t="s">
+        <v>98</v>
+      </c>
+      <c r="AF66">
         <v>4583</v>
       </c>
-      <c r="AE66">
+      <c r="AG66">
         <v>67</v>
       </c>
-      <c r="AF66">
-        <v>0</v>
-      </c>
-      <c r="AG66">
+      <c r="AH66">
+        <v>0</v>
+      </c>
+      <c r="AI66">
         <v>4516</v>
       </c>
     </row>
-    <row r="67" spans="1:33">
+    <row r="67" spans="1:35">
       <c r="A67" s="1">
         <v>65</v>
       </c>
@@ -7485,23 +7899,29 @@
       <c r="AB67">
         <v>65</v>
       </c>
-      <c r="AC67" t="s">
-        <v>97</v>
+      <c r="AC67">
+        <v>65</v>
       </c>
       <c r="AD67">
+        <v>65</v>
+      </c>
+      <c r="AE67" t="s">
+        <v>99</v>
+      </c>
+      <c r="AF67">
         <v>4632</v>
       </c>
-      <c r="AE67">
+      <c r="AG67">
         <v>69</v>
       </c>
-      <c r="AF67">
-        <v>0</v>
-      </c>
-      <c r="AG67">
+      <c r="AH67">
+        <v>0</v>
+      </c>
+      <c r="AI67">
         <v>4563</v>
       </c>
     </row>
-    <row r="68" spans="1:33">
+    <row r="68" spans="1:35">
       <c r="A68" s="1">
         <v>66</v>
       </c>
@@ -7586,23 +8006,29 @@
       <c r="AB68">
         <v>66</v>
       </c>
-      <c r="AC68" t="s">
-        <v>98</v>
+      <c r="AC68">
+        <v>66</v>
       </c>
       <c r="AD68">
+        <v>66</v>
+      </c>
+      <c r="AE68" t="s">
+        <v>100</v>
+      </c>
+      <c r="AF68">
         <v>4682</v>
       </c>
-      <c r="AE68">
+      <c r="AG68">
         <v>70</v>
       </c>
-      <c r="AF68">
-        <v>0</v>
-      </c>
-      <c r="AG68">
+      <c r="AH68">
+        <v>0</v>
+      </c>
+      <c r="AI68">
         <v>4612</v>
       </c>
     </row>
-    <row r="69" spans="1:33">
+    <row r="69" spans="1:35">
       <c r="A69" s="1">
         <v>67</v>
       </c>
@@ -7687,23 +8113,29 @@
       <c r="AB69">
         <v>67</v>
       </c>
-      <c r="AC69" t="s">
-        <v>99</v>
+      <c r="AC69">
+        <v>67</v>
       </c>
       <c r="AD69">
+        <v>67</v>
+      </c>
+      <c r="AE69" t="s">
+        <v>101</v>
+      </c>
+      <c r="AF69">
         <v>4806</v>
       </c>
-      <c r="AE69">
+      <c r="AG69">
         <v>70</v>
       </c>
-      <c r="AF69">
-        <v>0</v>
-      </c>
-      <c r="AG69">
+      <c r="AH69">
+        <v>0</v>
+      </c>
+      <c r="AI69">
         <v>4736</v>
       </c>
     </row>
-    <row r="70" spans="1:33">
+    <row r="70" spans="1:35">
       <c r="A70" s="1">
         <v>68</v>
       </c>
@@ -7788,23 +8220,29 @@
       <c r="AB70">
         <v>68</v>
       </c>
-      <c r="AC70" t="s">
-        <v>100</v>
+      <c r="AC70">
+        <v>68</v>
       </c>
       <c r="AD70">
+        <v>68</v>
+      </c>
+      <c r="AE70" t="s">
+        <v>102</v>
+      </c>
+      <c r="AF70">
         <v>4994</v>
       </c>
-      <c r="AE70">
+      <c r="AG70">
         <v>71</v>
       </c>
-      <c r="AF70">
-        <v>0</v>
-      </c>
-      <c r="AG70">
+      <c r="AH70">
+        <v>0</v>
+      </c>
+      <c r="AI70">
         <v>4923</v>
       </c>
     </row>
-    <row r="71" spans="1:33">
+    <row r="71" spans="1:35">
       <c r="A71" s="1">
         <v>69</v>
       </c>
@@ -7889,23 +8327,29 @@
       <c r="AB71">
         <v>69</v>
       </c>
-      <c r="AC71" t="s">
-        <v>101</v>
+      <c r="AC71">
+        <v>69</v>
       </c>
       <c r="AD71">
+        <v>69</v>
+      </c>
+      <c r="AE71" t="s">
+        <v>103</v>
+      </c>
+      <c r="AF71">
         <v>5118</v>
       </c>
-      <c r="AE71">
+      <c r="AG71">
         <v>74</v>
       </c>
-      <c r="AF71">
-        <v>0</v>
-      </c>
-      <c r="AG71">
+      <c r="AH71">
+        <v>0</v>
+      </c>
+      <c r="AI71">
         <v>5044</v>
       </c>
     </row>
-    <row r="72" spans="1:33">
+    <row r="72" spans="1:35">
       <c r="A72" s="1">
         <v>70</v>
       </c>
@@ -7990,23 +8434,29 @@
       <c r="AB72">
         <v>70</v>
       </c>
-      <c r="AC72" t="s">
-        <v>102</v>
+      <c r="AC72">
+        <v>70</v>
       </c>
       <c r="AD72">
+        <v>70</v>
+      </c>
+      <c r="AE72" t="s">
+        <v>104</v>
+      </c>
+      <c r="AF72">
         <v>5242</v>
       </c>
-      <c r="AE72">
+      <c r="AG72">
         <v>74</v>
       </c>
-      <c r="AF72">
-        <v>0</v>
-      </c>
-      <c r="AG72">
+      <c r="AH72">
+        <v>0</v>
+      </c>
+      <c r="AI72">
         <v>5168</v>
       </c>
     </row>
-    <row r="73" spans="1:33">
+    <row r="73" spans="1:35">
       <c r="A73" s="1">
         <v>71</v>
       </c>
@@ -8091,23 +8541,29 @@
       <c r="AB73">
         <v>71</v>
       </c>
-      <c r="AC73" t="s">
-        <v>103</v>
+      <c r="AC73">
+        <v>71</v>
       </c>
       <c r="AD73">
+        <v>71</v>
+      </c>
+      <c r="AE73" t="s">
+        <v>105</v>
+      </c>
+      <c r="AF73">
         <v>5340</v>
       </c>
-      <c r="AE73">
+      <c r="AG73">
         <v>74</v>
       </c>
-      <c r="AF73">
-        <v>0</v>
-      </c>
-      <c r="AG73">
+      <c r="AH73">
+        <v>0</v>
+      </c>
+      <c r="AI73">
         <v>5266</v>
       </c>
     </row>
-    <row r="74" spans="1:33">
+    <row r="74" spans="1:35">
       <c r="A74" s="1">
         <v>72</v>
       </c>
@@ -8192,23 +8648,29 @@
       <c r="AB74">
         <v>72</v>
       </c>
-      <c r="AC74" t="s">
-        <v>104</v>
+      <c r="AC74">
+        <v>72</v>
       </c>
       <c r="AD74">
+        <v>72</v>
+      </c>
+      <c r="AE74" t="s">
+        <v>106</v>
+      </c>
+      <c r="AF74">
         <v>5449</v>
       </c>
-      <c r="AE74">
+      <c r="AG74">
         <v>74</v>
       </c>
-      <c r="AF74">
-        <v>0</v>
-      </c>
-      <c r="AG74">
+      <c r="AH74">
+        <v>0</v>
+      </c>
+      <c r="AI74">
         <v>5375</v>
       </c>
     </row>
-    <row r="75" spans="1:33">
+    <row r="75" spans="1:35">
       <c r="A75" s="1">
         <v>73</v>
       </c>
@@ -8293,23 +8755,29 @@
       <c r="AB75">
         <v>73</v>
       </c>
-      <c r="AC75" t="s">
-        <v>105</v>
+      <c r="AC75">
+        <v>73</v>
       </c>
       <c r="AD75">
+        <v>73</v>
+      </c>
+      <c r="AE75" t="s">
+        <v>107</v>
+      </c>
+      <c r="AF75">
         <v>5603</v>
       </c>
-      <c r="AE75">
+      <c r="AG75">
         <v>78</v>
       </c>
-      <c r="AF75">
-        <v>0</v>
-      </c>
-      <c r="AG75">
+      <c r="AH75">
+        <v>0</v>
+      </c>
+      <c r="AI75">
         <v>5525</v>
       </c>
     </row>
-    <row r="76" spans="1:33">
+    <row r="76" spans="1:35">
       <c r="A76" s="1">
         <v>74</v>
       </c>
@@ -8394,23 +8862,29 @@
       <c r="AB76">
         <v>74</v>
       </c>
-      <c r="AC76" t="s">
-        <v>106</v>
+      <c r="AC76">
+        <v>74</v>
       </c>
       <c r="AD76">
+        <v>74</v>
+      </c>
+      <c r="AE76" t="s">
+        <v>108</v>
+      </c>
+      <c r="AF76">
         <v>5756</v>
       </c>
-      <c r="AE76">
+      <c r="AG76">
         <v>78</v>
       </c>
-      <c r="AF76">
-        <v>0</v>
-      </c>
-      <c r="AG76">
+      <c r="AH76">
+        <v>0</v>
+      </c>
+      <c r="AI76">
         <v>5678</v>
       </c>
     </row>
-    <row r="77" spans="1:33">
+    <row r="77" spans="1:35">
       <c r="A77" s="1">
         <v>75</v>
       </c>
@@ -8495,23 +8969,29 @@
       <c r="AB77">
         <v>75</v>
       </c>
-      <c r="AC77" t="s">
-        <v>107</v>
+      <c r="AC77">
+        <v>75</v>
       </c>
       <c r="AD77">
+        <v>75</v>
+      </c>
+      <c r="AE77" t="s">
+        <v>109</v>
+      </c>
+      <c r="AF77">
         <v>5901</v>
       </c>
-      <c r="AE77">
+      <c r="AG77">
         <v>81</v>
       </c>
-      <c r="AF77">
-        <v>0</v>
-      </c>
-      <c r="AG77">
+      <c r="AH77">
+        <v>0</v>
+      </c>
+      <c r="AI77">
         <v>5820</v>
       </c>
     </row>
-    <row r="78" spans="1:33">
+    <row r="78" spans="1:35">
       <c r="A78" s="1">
         <v>76</v>
       </c>
@@ -8596,23 +9076,29 @@
       <c r="AB78">
         <v>76</v>
       </c>
-      <c r="AC78" t="s">
-        <v>108</v>
+      <c r="AC78">
+        <v>76</v>
       </c>
       <c r="AD78">
+        <v>76</v>
+      </c>
+      <c r="AE78" t="s">
+        <v>110</v>
+      </c>
+      <c r="AF78">
         <v>6086</v>
       </c>
-      <c r="AE78">
+      <c r="AG78">
         <v>81</v>
       </c>
-      <c r="AF78">
-        <v>0</v>
-      </c>
-      <c r="AG78">
+      <c r="AH78">
+        <v>0</v>
+      </c>
+      <c r="AI78">
         <v>6005</v>
       </c>
     </row>
-    <row r="79" spans="1:33">
+    <row r="79" spans="1:35">
       <c r="A79" s="1">
         <v>77</v>
       </c>
@@ -8697,23 +9183,29 @@
       <c r="AB79">
         <v>77</v>
       </c>
-      <c r="AC79" t="s">
-        <v>109</v>
+      <c r="AC79">
+        <v>77</v>
       </c>
       <c r="AD79">
+        <v>77</v>
+      </c>
+      <c r="AE79" t="s">
+        <v>111</v>
+      </c>
+      <c r="AF79">
         <v>6182</v>
       </c>
-      <c r="AE79">
+      <c r="AG79">
         <v>81</v>
       </c>
-      <c r="AF79">
-        <v>0</v>
-      </c>
-      <c r="AG79">
+      <c r="AH79">
+        <v>0</v>
+      </c>
+      <c r="AI79">
         <v>6101</v>
       </c>
     </row>
-    <row r="80" spans="1:33">
+    <row r="80" spans="1:35">
       <c r="A80" s="1">
         <v>78</v>
       </c>
@@ -8798,23 +9290,29 @@
       <c r="AB80">
         <v>78</v>
       </c>
-      <c r="AC80" t="s">
-        <v>110</v>
+      <c r="AC80">
+        <v>78</v>
       </c>
       <c r="AD80">
+        <v>78</v>
+      </c>
+      <c r="AE80" t="s">
+        <v>112</v>
+      </c>
+      <c r="AF80">
         <v>6296</v>
       </c>
-      <c r="AE80">
+      <c r="AG80">
         <v>83</v>
       </c>
-      <c r="AF80">
-        <v>0</v>
-      </c>
-      <c r="AG80">
+      <c r="AH80">
+        <v>0</v>
+      </c>
+      <c r="AI80">
         <v>6213</v>
       </c>
     </row>
-    <row r="81" spans="1:33">
+    <row r="81" spans="1:35">
       <c r="A81" s="1">
         <v>79</v>
       </c>
@@ -8899,23 +9397,29 @@
       <c r="AB81">
         <v>79</v>
       </c>
-      <c r="AC81" t="s">
-        <v>111</v>
+      <c r="AC81">
+        <v>79</v>
       </c>
       <c r="AD81">
+        <v>79</v>
+      </c>
+      <c r="AE81" t="s">
+        <v>113</v>
+      </c>
+      <c r="AF81">
         <v>6421</v>
       </c>
-      <c r="AE81">
+      <c r="AG81">
         <v>85</v>
       </c>
-      <c r="AF81">
-        <v>0</v>
-      </c>
-      <c r="AG81">
+      <c r="AH81">
+        <v>0</v>
+      </c>
+      <c r="AI81">
         <v>6336</v>
       </c>
     </row>
-    <row r="82" spans="1:33">
+    <row r="82" spans="1:35">
       <c r="A82" s="1">
         <v>80</v>
       </c>
@@ -9000,23 +9504,29 @@
       <c r="AB82">
         <v>80</v>
       </c>
-      <c r="AC82" t="s">
-        <v>112</v>
+      <c r="AC82">
+        <v>80</v>
       </c>
       <c r="AD82">
+        <v>80</v>
+      </c>
+      <c r="AE82" t="s">
+        <v>114</v>
+      </c>
+      <c r="AF82">
         <v>6591</v>
       </c>
-      <c r="AE82">
+      <c r="AG82">
         <v>85</v>
       </c>
-      <c r="AF82">
-        <v>0</v>
-      </c>
-      <c r="AG82">
+      <c r="AH82">
+        <v>0</v>
+      </c>
+      <c r="AI82">
         <v>6506</v>
       </c>
     </row>
-    <row r="83" spans="1:33">
+    <row r="83" spans="1:35">
       <c r="A83" s="1">
         <v>81</v>
       </c>
@@ -9101,23 +9611,29 @@
       <c r="AB83">
         <v>81</v>
       </c>
-      <c r="AC83" t="s">
-        <v>113</v>
+      <c r="AC83">
+        <v>81</v>
       </c>
       <c r="AD83">
+        <v>81</v>
+      </c>
+      <c r="AE83" t="s">
+        <v>115</v>
+      </c>
+      <c r="AF83">
         <v>6776</v>
       </c>
-      <c r="AE83">
+      <c r="AG83">
         <v>87</v>
       </c>
-      <c r="AF83">
-        <v>0</v>
-      </c>
-      <c r="AG83">
+      <c r="AH83">
+        <v>0</v>
+      </c>
+      <c r="AI83">
         <v>6689</v>
       </c>
     </row>
-    <row r="84" spans="1:33">
+    <row r="84" spans="1:35">
       <c r="A84" s="1">
         <v>82</v>
       </c>
@@ -9163,23 +9679,29 @@
       <c r="O84">
         <v>82</v>
       </c>
-      <c r="AC84" t="s">
-        <v>114</v>
-      </c>
-      <c r="AD84">
+      <c r="P84">
+        <v>82</v>
+      </c>
+      <c r="Q84">
+        <v>82</v>
+      </c>
+      <c r="AE84" t="s">
+        <v>116</v>
+      </c>
+      <c r="AF84">
         <v>6942</v>
       </c>
-      <c r="AE84">
+      <c r="AG84">
         <v>93</v>
       </c>
-      <c r="AF84">
-        <v>0</v>
-      </c>
-      <c r="AG84">
+      <c r="AH84">
+        <v>0</v>
+      </c>
+      <c r="AI84">
         <v>6849</v>
       </c>
     </row>
-    <row r="85" spans="1:33">
+    <row r="85" spans="1:35">
       <c r="A85" s="1">
         <v>83</v>
       </c>
@@ -9216,23 +9738,29 @@
       <c r="L85">
         <v>83</v>
       </c>
-      <c r="AC85" t="s">
-        <v>115</v>
-      </c>
-      <c r="AD85">
+      <c r="M85">
+        <v>83</v>
+      </c>
+      <c r="N85">
+        <v>83</v>
+      </c>
+      <c r="AE85" t="s">
+        <v>117</v>
+      </c>
+      <c r="AF85">
         <v>7148</v>
       </c>
-      <c r="AE85">
+      <c r="AG85">
         <v>93</v>
       </c>
-      <c r="AF85">
-        <v>0</v>
-      </c>
-      <c r="AG85">
+      <c r="AH85">
+        <v>0</v>
+      </c>
+      <c r="AI85">
         <v>7055</v>
       </c>
     </row>
-    <row r="86" spans="1:33">
+    <row r="86" spans="1:35">
       <c r="A86" s="1">
         <v>84</v>
       </c>
@@ -9242,86 +9770,202 @@
       <c r="C86">
         <v>84</v>
       </c>
-      <c r="AC86" t="s">
-        <v>116</v>
-      </c>
-      <c r="AD86">
+      <c r="D86">
+        <v>84</v>
+      </c>
+      <c r="E86">
+        <v>84</v>
+      </c>
+      <c r="AE86" t="s">
+        <v>118</v>
+      </c>
+      <c r="AF86">
         <v>7309</v>
       </c>
-      <c r="AE86">
+      <c r="AG86">
         <v>93</v>
       </c>
-      <c r="AF86">
-        <v>0</v>
-      </c>
-      <c r="AG86">
+      <c r="AH86">
+        <v>0</v>
+      </c>
+      <c r="AI86">
         <v>7216</v>
       </c>
     </row>
-    <row r="87" spans="1:33">
+    <row r="87" spans="1:35">
       <c r="A87" s="1">
         <v>85</v>
       </c>
       <c r="B87">
         <v>85</v>
       </c>
-      <c r="AC87" t="s">
-        <v>117</v>
-      </c>
-      <c r="AD87">
+      <c r="C87">
+        <v>85</v>
+      </c>
+      <c r="D87">
+        <v>85</v>
+      </c>
+      <c r="AE87" t="s">
+        <v>119</v>
+      </c>
+      <c r="AF87">
         <v>7468</v>
       </c>
-      <c r="AE87">
+      <c r="AG87">
         <v>94</v>
       </c>
-      <c r="AF87">
-        <v>0</v>
-      </c>
-      <c r="AG87">
+      <c r="AH87">
+        <v>0</v>
+      </c>
+      <c r="AI87">
         <v>7374</v>
       </c>
     </row>
-    <row r="88" spans="1:33">
+    <row r="88" spans="1:35">
       <c r="A88" s="1">
         <v>86</v>
       </c>
       <c r="B88">
         <v>86</v>
       </c>
-      <c r="AC88" t="s">
-        <v>118</v>
-      </c>
-      <c r="AD88">
+      <c r="C88">
+        <v>86</v>
+      </c>
+      <c r="D88">
+        <v>86</v>
+      </c>
+      <c r="AE88" t="s">
+        <v>120</v>
+      </c>
+      <c r="AF88">
         <v>7616</v>
       </c>
-      <c r="AE88">
+      <c r="AG88">
         <v>96</v>
       </c>
-      <c r="AF88">
-        <v>0</v>
-      </c>
-      <c r="AG88">
+      <c r="AH88">
+        <v>0</v>
+      </c>
+      <c r="AI88">
         <v>7520</v>
       </c>
     </row>
-    <row r="89" spans="1:33">
+    <row r="89" spans="1:35">
       <c r="A89" s="1">
         <v>87</v>
       </c>
-      <c r="AC89" t="s">
-        <v>119</v>
-      </c>
-      <c r="AD89">
+      <c r="B89">
+        <v>87</v>
+      </c>
+      <c r="C89">
+        <v>87</v>
+      </c>
+      <c r="AE89" t="s">
+        <v>121</v>
+      </c>
+      <c r="AF89">
         <v>7809</v>
       </c>
-      <c r="AE89">
+      <c r="AG89">
         <v>99</v>
       </c>
-      <c r="AF89">
-        <v>0</v>
-      </c>
-      <c r="AG89">
+      <c r="AH89">
+        <v>0</v>
+      </c>
+      <c r="AI89">
         <v>7710</v>
+      </c>
+    </row>
+    <row r="90" spans="1:35">
+      <c r="A90" s="1">
+        <v>88</v>
+      </c>
+      <c r="B90">
+        <v>88</v>
+      </c>
+      <c r="AE90" t="s">
+        <v>122</v>
+      </c>
+      <c r="AF90">
+        <v>8083</v>
+      </c>
+      <c r="AG90">
+        <v>100</v>
+      </c>
+      <c r="AH90">
+        <v>0</v>
+      </c>
+      <c r="AI90">
+        <v>7983</v>
+      </c>
+    </row>
+    <row r="91" spans="1:35">
+      <c r="A91" s="1">
+        <v>89</v>
+      </c>
+      <c r="B91">
+        <v>89</v>
+      </c>
+      <c r="AE91" t="s">
+        <v>123</v>
+      </c>
+      <c r="AF91">
+        <v>8363</v>
+      </c>
+      <c r="AG91">
+        <v>102</v>
+      </c>
+      <c r="AH91">
+        <v>0</v>
+      </c>
+      <c r="AI91">
+        <v>8261</v>
+      </c>
+    </row>
+    <row r="92" spans="1:35">
+      <c r="A92" s="1">
+        <v>90</v>
+      </c>
+      <c r="B92">
+        <v>90</v>
+      </c>
+      <c r="AE92" t="s">
+        <v>124</v>
+      </c>
+      <c r="AF92">
+        <v>8687</v>
+      </c>
+      <c r="AG92">
+        <v>102</v>
+      </c>
+      <c r="AH92">
+        <v>0</v>
+      </c>
+      <c r="AI92">
+        <v>8585</v>
+      </c>
+    </row>
+    <row r="93" spans="1:35">
+      <c r="A93" s="1">
+        <v>91</v>
+      </c>
+      <c r="B93">
+        <v>91</v>
+      </c>
+      <c r="AE93" t="s">
+        <v>125</v>
+      </c>
+      <c r="AF93">
+        <v>8878</v>
+      </c>
+      <c r="AG93">
+        <v>102</v>
+      </c>
+      <c r="AH93">
+        <v>0</v>
+      </c>
+      <c r="AI93">
+        <v>8776</v>
       </c>
     </row>
   </sheetData>

</xml_diff>